<commit_message>
Write initial code for replacing values below the LOD, clean up R directory
</commit_message>
<xml_diff>
--- a/inst/extdata/LOD_values.xlsx
+++ b/inst/extdata/LOD_values.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Notes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="31">
   <si>
     <t>Parameter</t>
   </si>
@@ -76,9 +77,6 @@
     <t>SiO2</t>
   </si>
   <si>
-    <t>mgSiO2</t>
-  </si>
-  <si>
     <t>SC_L</t>
   </si>
   <si>
@@ -92,15 +90,47 @@
   </si>
   <si>
     <t>Chla</t>
+  </si>
+  <si>
+    <t>Sheet 1 may be updated to reflect the most recent years LOD/LOQ values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Currently the "lod_checkdata" internal dataframe is shown in red. Contact DaveA to update. </t>
+  </si>
+  <si>
+    <t>Rows may be added to accommodate additional parameters as needed, however, the internal check will error when rows are added until the "lod_checkdata" is updated internally, or may optionally be temporarily added using the "add_lod_row" argument to the format_sampleMaster function</t>
+  </si>
+  <si>
+    <t>Alk</t>
+  </si>
+  <si>
+    <t>pH_L</t>
+  </si>
+  <si>
+    <t>pH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -127,8 +157,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,12 +641,12 @@
         <v>1.2</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14">
         <v>10</v>
@@ -623,12 +655,12 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15">
         <v>11</v>
@@ -642,7 +674,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16">
         <v>11</v>
@@ -656,7 +688,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17">
         <v>0.1</v>
@@ -666,10 +698,210 @@
       </c>
       <c r="D17" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AA7" sqref="AA7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>